<commit_message>
Fixing errors and bugs to handle multiple inputs
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Manufacturer/Supplier</t>
   </si>
@@ -31,13 +31,25 @@
     <t>OM</t>
   </si>
   <si>
-    <t>JG-MS-8004</t>
+    <t>NC-NTH-8009</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>https://barcode.tec-it.com/barcode.ashx?data=OM-NC-NTH-8009-R1</t>
+  </si>
+  <si>
+    <t>DIPSHI</t>
+  </si>
+  <si>
+    <t>NC-NK-9005</t>
   </si>
   <si>
     <t>R2</t>
   </si>
   <si>
-    <t>https://barcode.tec-it.com/barcode.ashx?data=OM-JG-MS-8004-R2</t>
+    <t>https://barcode.tec-it.com/barcode.ashx?data=DIPSHI-NC-NK-9005-R2</t>
   </si>
 </sst>
 </file>
@@ -382,7 +394,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -416,9 +428,24 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>